<commit_message>
report, post invalid article,, done
</commit_message>
<xml_diff>
--- a/files/APItest/article/PostArticleTest.xlsx
+++ b/files/APItest/article/PostArticleTest.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\APItest\conduittests\article\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\APItest\article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C5173C-5303-448B-AD52-A338AFDEE34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63D5CCE-FDD4-484C-A751-98495EC9CBE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A3DFE-CDA4-4F07-8DD2-7B17F915E2D5}"/>
   </bookViews>
   <sheets>
     <sheet name="postNewArticleTest" sheetId="1" r:id="rId1"/>
+    <sheet name="postNewInvalidArticleTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
   <si>
     <t>Run</t>
   </si>
@@ -39,9 +40,6 @@
     <t>Article Title</t>
   </si>
   <si>
-    <t>What's this article about?</t>
-  </si>
-  <si>
     <t>Write your article (body)</t>
   </si>
   <si>
@@ -91,13 +89,57 @@
   </si>
   <si>
     <t>123456789</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>expected response</t>
+  </si>
+  <si>
+    <t>expected status code</t>
+  </si>
+  <si>
+    <t>{
+    "errors": {
+        "description": [
+            "can't be blank",
+            "is too short (minimum is 1 character)"
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "errors": {
+        "title": [
+            "can't be blank",
+            "is too short (minimum is 1 character)"
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "errors": {
+        "body": [
+            "can't be blank"
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>test case number 4</t>
+  </si>
+  <si>
+    <t>test case number 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +159,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,13 +192,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EEE2E0F-A3AB-45B8-BA3C-BF3BA838A58C}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,107 +553,327 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57321BF3-A261-40FC-A84F-94EDBB595E0C}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="6">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="6">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="6">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all APIs are done
</commit_message>
<xml_diff>
--- a/files/APItest/article/PostArticleTest.xlsx
+++ b/files/APItest/article/PostArticleTest.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\APItest\article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63D5CCE-FDD4-484C-A751-98495EC9CBE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A212033-D311-4CEE-8576-C9CFB3E97DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{548A3DFE-CDA4-4F07-8DD2-7B17F915E2D5}"/>
   </bookViews>
   <sheets>
-    <sheet name="postNewArticleTest" sheetId="1" r:id="rId1"/>
-    <sheet name="postNewInvalidArticleTest" sheetId="2" r:id="rId2"/>
+    <sheet name="postValidArticleTest" sheetId="1" r:id="rId1"/>
+    <sheet name="postInvalidArticleTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
   <si>
     <t>Run</t>
   </si>
@@ -98,26 +98,6 @@
   </si>
   <si>
     <t>expected status code</t>
-  </si>
-  <si>
-    <t>{
-    "errors": {
-        "description": [
-            "can't be blank",
-            "is too short (minimum is 1 character)"
-        ]
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "errors": {
-        "title": [
-            "can't be blank",
-            "is too short (minimum is 1 character)"
-        ]
-    }
-}</t>
   </si>
   <si>
     <t>{
@@ -133,6 +113,27 @@
   </si>
   <si>
     <t>test case number 5</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>without title</t>
+  </si>
+  <si>
+    <t>{  "errors":  {  "title":  [  "can't be blank", "is too short (minimum is 1 character)"  ]  }  }</t>
+  </si>
+  <si>
+    <t>without  description</t>
+  </si>
+  <si>
+    <t>{ "errors": { "description": [ "can't be blank", "is too short (minimum is 1 character)" ] } }</t>
+  </si>
+  <si>
+    <t>without body</t>
+  </si>
+  <si>
+    <t>without body case 2</t>
   </si>
 </sst>
 </file>
@@ -192,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -210,6 +211,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,7 +529,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F2" sqref="F2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -690,7 +692,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -722,10 +724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57321BF3-A261-40FC-A84F-94EDBB595E0C}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,31 +745,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -778,101 +780,134 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
+      <c r="C2" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="K2" s="6">
         <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K3" s="6">
         <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K4" s="6">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="6">
         <v>422</v>
       </c>
     </row>

</xml_diff>